<commit_message>
Minor updates to HashtagsPerDay
</commit_message>
<xml_diff>
--- a/Analysis/HashtagsPerDay.xlsx
+++ b/Analysis/HashtagsPerDay.xlsx
@@ -91,7 +91,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -99,6 +99,7 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2853,10 +2854,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J370"/>
+  <dimension ref="A1:J371"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="A345" workbookViewId="0">
+      <selection activeCell="B371" sqref="B371"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -10271,6 +10272,9 @@
         <f t="shared" si="16"/>
         <v>75083</v>
       </c>
+    </row>
+    <row r="371" spans="1:6">
+      <c r="B371" s="5"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C3:C370">

</xml_diff>